<commit_message>
Created 4 Main Seprated Folder for excel, power bi, sql and python in main folder
</commit_message>
<xml_diff>
--- a/Certified Data Analyst 2024-2025 From Excel to Python - Master Data Analytics-Introduction-Structure-File.xlsx
+++ b/Certified Data Analyst 2024-2025 From Excel to Python - Master Data Analytics-Introduction-Structure-File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA Analytics Study data\Digital Analysis 3.0M\GitHub\Excel-Classes-Excel-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40695A1A-2888-4DB4-BE9C-8FB655532512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0882A2B-8FBC-4D5A-87D8-DF7D8DF84E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F6D9AFDF-A79F-445E-826E-10108AB2203E}"/>
   </bookViews>
@@ -284,7 +284,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,39 +608,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -658,8 +625,41 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1002,7 +1002,7 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4.75" customWidth="1"/>
     <col min="2" max="3" width="11.75" bestFit="1" customWidth="1"/>
@@ -1012,31 +1012,31 @@
     <col min="8" max="8" width="38.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="2:9" ht="14.25" customHeight="1">
+      <c r="B2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-    </row>
-    <row r="3" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+    </row>
+    <row r="3" spans="2:9" ht="24" customHeight="1">
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-    </row>
-    <row r="5" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+    </row>
+    <row r="5" spans="2:9" ht="15">
       <c r="G5" s="1">
         <v>1</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" ht="20.25">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="15">
       <c r="G7" s="1">
         <v>3</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="15">
       <c r="G8" s="1">
         <v>4</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="15">
       <c r="G9" s="1">
         <v>5</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="15">
       <c r="G10" s="1">
         <v>6</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="15">
       <c r="G11" s="1">
         <v>7</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="15">
       <c r="G12" s="1">
         <v>8</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="15">
       <c r="G13" s="1">
         <v>9</v>
       </c>
@@ -1134,11 +1134,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875815BF-FC94-41B2-AFE1-C7050D85F14D}">
   <dimension ref="B3:AN29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="3" max="3" width="35.375" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
@@ -1150,73 +1150,73 @@
     <col min="11" max="11" width="39.875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="52.75" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="2:40" ht="14.25" customHeight="1">
+      <c r="B3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
       <c r="F3" s="16"/>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="J3" s="17" t="s">
+      <c r="H3" s="25"/>
+      <c r="J3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="N3" s="17" t="s">
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="N3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="R3" s="17" t="s">
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="R3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-    </row>
-    <row r="4" spans="2:40" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+    </row>
+    <row r="4" spans="2:40" ht="21.75" customHeight="1">
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="16"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
       <c r="AN4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="O5" s="35" t="s">
+    <row r="5" spans="2:40">
+      <c r="O5" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="P5" s="35"/>
-    </row>
-    <row r="6" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="33"/>
+    </row>
+    <row r="6" spans="2:40" ht="14.25" customHeight="1">
       <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="7" t="s">
         <v>13</v>
       </c>
@@ -1229,22 +1229,22 @@
       <c r="J6">
         <v>1</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="35" t="s">
+      <c r="O6" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="P6" s="35"/>
-    </row>
-    <row r="7" spans="2:40" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P6" s="33"/>
+    </row>
+    <row r="7" spans="2:40" ht="15.75">
       <c r="B7" s="8">
         <v>1</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="24"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="11" t="s">
         <v>15</v>
       </c>
@@ -1254,22 +1254,22 @@
       <c r="H7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="28" t="s">
+      <c r="L7" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="O7" s="35" t="s">
+      <c r="O7" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="P7" s="35"/>
-    </row>
-    <row r="8" spans="2:40" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P7" s="33"/>
+    </row>
+    <row r="8" spans="2:40" ht="15.75">
       <c r="B8" s="9">
         <v>2</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="12" t="s">
         <v>14</v>
       </c>
@@ -1279,245 +1279,252 @@
       <c r="H8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="31" t="s">
+      <c r="L8" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:40" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:40" ht="15.75">
       <c r="B9" s="8">
         <v>3</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="11" t="s">
         <v>14</v>
       </c>
       <c r="J9">
         <v>2</v>
       </c>
-      <c r="K9" s="30" t="s">
+      <c r="K9" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="L9" s="28"/>
-      <c r="O9" s="32" t="s">
+      <c r="L9" s="17"/>
+      <c r="O9" s="21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="2:40" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:40" ht="15.75">
       <c r="B10" s="9">
         <v>4</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="25"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="30"/>
-      <c r="L10" s="28" t="s">
+      <c r="I10" s="19"/>
+      <c r="L10" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="P10" s="28" t="s">
+      <c r="P10" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="2:40" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:40" ht="15.75">
       <c r="B11" s="8">
         <v>5</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="24"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="28" t="s">
+      <c r="L11" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="28" t="s">
+      <c r="P11" s="17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="2:40" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:40" ht="15.75">
       <c r="B12" s="9">
         <v>6</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="25"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="28" t="s">
+      <c r="L12" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="O12" s="29" t="s">
+      <c r="O12" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="2:40" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:40" ht="15.75">
       <c r="B13" s="10"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
       <c r="E13" s="13"/>
-      <c r="L13" s="28" t="s">
+      <c r="L13" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28" t="s">
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="L14" s="28" t="s">
+    <row r="14" spans="2:40">
+      <c r="L14" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="P14" s="28" t="s">
+      <c r="P14" s="17" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="2:40" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:40" ht="15">
       <c r="J15">
         <v>3</v>
       </c>
-      <c r="K15" s="30" t="s">
+      <c r="K15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="L15" s="31"/>
-      <c r="P15" s="34" t="s">
+      <c r="L15" s="20"/>
+      <c r="P15" s="23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="L16" s="28" t="s">
+    <row r="16" spans="2:40">
+      <c r="L16" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="P16" s="34" t="s">
+      <c r="P16" s="23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="10:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="L17" s="28" t="s">
+    <row r="17" spans="10:16" ht="15">
+      <c r="L17" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="O17" s="29" t="s">
+      <c r="O17" s="18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="L18" s="28" t="s">
+    <row r="18" spans="10:16">
+      <c r="L18" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="P18" s="28" t="s">
+      <c r="P18" s="17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="10:16" ht="15">
       <c r="J19">
         <v>4</v>
       </c>
-      <c r="K19" s="30" t="s">
+      <c r="K19" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="L19" s="31"/>
-      <c r="P19" s="33" t="s">
+      <c r="L19" s="20"/>
+      <c r="P19" s="22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="10:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L20" s="28" t="s">
+    <row r="20" spans="10:16" ht="15">
+      <c r="L20" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="O20" s="32" t="s">
+      <c r="O20" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="L21" s="31" t="s">
+    <row r="21" spans="10:16">
+      <c r="L21" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="P21" s="28" t="s">
+      <c r="P21" s="17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="L22" s="28" t="s">
+    <row r="22" spans="10:16">
+      <c r="L22" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="P22" s="28" t="s">
+      <c r="P22" s="17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="10:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="L23" s="28" t="s">
+    <row r="23" spans="10:16" ht="15">
+      <c r="L23" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="O23" s="32" t="s">
+      <c r="O23" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="10:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="10:16" ht="15">
       <c r="J24">
         <v>5</v>
       </c>
-      <c r="K24" s="30" t="s">
+      <c r="K24" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="L24" s="31"/>
-      <c r="P24" s="28" t="s">
+      <c r="L24" s="20"/>
+      <c r="P24" s="17" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="L25" s="28" t="s">
+    <row r="25" spans="10:16">
+      <c r="L25" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="P25" s="28" t="s">
+      <c r="P25" s="17" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="10:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="L26" s="28" t="s">
+    <row r="26" spans="10:16" ht="15">
+      <c r="L26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="O26" s="29" t="s">
+      <c r="O26" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="10:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="10:16" ht="15">
       <c r="J27">
         <v>6</v>
       </c>
-      <c r="K27" s="30" t="s">
+      <c r="K27" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="L27" s="31"/>
-      <c r="P27" s="28" t="s">
+      <c r="L27" s="20"/>
+      <c r="P27" s="17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="10:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="L28" s="28" t="s">
+    <row r="28" spans="10:16" ht="15">
+      <c r="L28" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="O28" s="29" t="s">
+      <c r="O28" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="L29" s="28" t="s">
+    <row r="29" spans="10:16">
+      <c r="L29" s="17" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B3:E4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="J3:L4"/>
     <mergeCell ref="N3:P4"/>
     <mergeCell ref="R3:T4"/>
@@ -1527,13 +1534,6 @@
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O7:P7"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B3:E4"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1545,7 +1545,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1557,7 +1557,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1569,9 +1569,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>16</v>
       </c>

</xml_diff>